<commit_message>
Zapoceta implementacija administratorskih funkcionalnosti
</commit_message>
<xml_diff>
--- a/documentation/sbnz.xlsx
+++ b/documentation/sbnz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacji\OneDrive - uns.ac.rs\OSMI\Projects\dermatology_assistant\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEC4B1E-B62B-4034-A7F2-6902BBBC2EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1264A624-126A-45A8-A622-7A94E661660A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="235" xr2:uid="{8F260C12-4A40-47C1-8C81-EADC4A2AF9A1}"/>
+    <workbookView xWindow="0" yWindow="1335" windowWidth="21600" windowHeight="11385" tabRatio="235" firstSheet="1" activeTab="1" xr2:uid="{8F260C12-4A40-47C1-8C81-EADC4A2AF9A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
   <si>
     <t>Skin issues</t>
   </si>
@@ -347,6 +347,21 @@
     <t>Hyperpigmentation
 Dark spots, 
 Age spots</t>
+  </si>
+  <si>
+    <t>Atopic dermatitis</t>
+  </si>
+  <si>
+    <t>peeling</t>
+  </si>
+  <si>
+    <t>swelling</t>
+  </si>
+  <si>
+    <t>itching</t>
+  </si>
+  <si>
+    <t>burning</t>
   </si>
 </sst>
 </file>
@@ -651,7 +666,10 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="26">
+    <dxf>
+      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -673,42 +691,93 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="2" tint="-0.499984740745262"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="2" tint="-0.499984740745262"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="2" tint="-0.499984740745262"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="2" tint="-0.499984740745262"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -723,80 +792,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="2" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="2" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="2" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="2" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -829,7 +824,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{11E7AE69-BF09-437A-9A1B-2CF6726A2CB0}" name="Table8" displayName="Table8" ref="B3:G6" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{11E7AE69-BF09-437A-9A1B-2CF6726A2CB0}" name="Table8" displayName="Table8" ref="B3:G6" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24">
   <autoFilter ref="B3:G6" xr:uid="{5202518E-D7ED-4265-8561-6BC799949CA0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -839,12 +834,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{54FA025D-2FDA-4FE1-9818-C886BF17E8D9}" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B7F62EA9-A6EB-4F5A-A97D-868D167DAA67}" name="Skin issues" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{54FA025D-2FDA-4FE1-9818-C886BF17E8D9}" name="Name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B7F62EA9-A6EB-4F5A-A97D-868D167DAA67}" name="Skin issues" dataDxfId="22"/>
     <tableColumn id="3" xr3:uid="{1EBF7F4D-E945-4DB5-AF82-246ED1DAF0A8}" name="No of skin issues"/>
-    <tableColumn id="4" xr3:uid="{81046262-E5AD-4101-9A27-BD7EF511255E}" name="Not good for" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{27A6ABA8-B2B1-401E-A13C-43B85A44779A}" name="Best for age groups" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{7E9FE92C-0AC4-402F-A455-7F00240ADEE7}" name="Best for environment" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{81046262-E5AD-4101-9A27-BD7EF511255E}" name="Not good for" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{27A6ABA8-B2B1-401E-A13C-43B85A44779A}" name="Best for age groups" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{7E9FE92C-0AC4-402F-A455-7F00240ADEE7}" name="Best for environment" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -861,12 +856,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8F740844-6E19-47C9-800B-05BFF79813E2}" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{41819D2A-4828-4BA4-BB5C-EF3A643AF6B0}" name="Skin issues" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{8F740844-6E19-47C9-800B-05BFF79813E2}" name="Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{41819D2A-4828-4BA4-BB5C-EF3A643AF6B0}" name="Skin issues" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{E7545BE4-E81A-4541-B077-5805DCF5C1AD}" name="No of skin issues"/>
     <tableColumn id="4" xr3:uid="{2D9FBC91-C45B-4474-8E32-8785FCF10159}" name="Not good for" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{1B024E66-8930-47FF-9CC6-482B9CB47835}" name="Best for age groups" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{B54A3BBE-3018-4F3E-A5A2-FC4B6DB5BCD7}" name="Best for environment" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1B024E66-8930-47FF-9CC6-482B9CB47835}" name="Best for age groups" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{B54A3BBE-3018-4F3E-A5A2-FC4B6DB5BCD7}" name="Best for environment" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -883,12 +878,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D3164C07-BEB2-4FCC-B4B6-22C336132EC0}" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{9BC07E4D-A121-42AF-A4BD-E8E87B611290}" name="Skin issues" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{D3164C07-BEB2-4FCC-B4B6-22C336132EC0}" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{9BC07E4D-A121-42AF-A4BD-E8E87B611290}" name="Skin issues" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{9ED8B4E0-EE89-43C1-AB56-E37D2BEC7E5D}" name="No of skin issues"/>
-    <tableColumn id="4" xr3:uid="{10D67B87-79FF-42AF-BF42-D407CA4DE29B}" name="Not good for" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{0B00D4D7-04BF-49F5-B4AC-10A221FB98F8}" name="Best for age groups" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{5F73FE72-CB1A-4EDE-8CF7-7EE44A6AB385}" name="Best for environment" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{10D67B87-79FF-42AF-BF42-D407CA4DE29B}" name="Not good for" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{0B00D4D7-04BF-49F5-B4AC-10A221FB98F8}" name="Best for age groups" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{5F73FE72-CB1A-4EDE-8CF7-7EE44A6AB385}" name="Best for environment" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -905,12 +900,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E2D456E1-C237-4A46-B47A-E44B6AD953DA}" name="Name" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F0231537-CE32-46B9-A541-2F32286B21A6}" name="Skin issues" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{58596DA1-A922-430A-958E-C731A93F1E1E}" name="No of skin issues" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{E2D456E1-C237-4A46-B47A-E44B6AD953DA}" name="Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F0231537-CE32-46B9-A541-2F32286B21A6}" name="Skin issues" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{58596DA1-A922-430A-958E-C731A93F1E1E}" name="No of skin issues" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{F8243A82-0CF2-4F56-AAA7-B6E7504C8546}" name="Not good for" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{0CBC2AB6-68A7-4FFA-9E93-7B9CCFBA67D9}" name="Best for age groups" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{15C501EB-9E24-4CAB-907B-4A5E7B3E6815}" name="Best for environment" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{0CBC2AB6-68A7-4FFA-9E93-7B9CCFBA67D9}" name="Best for age groups" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{15C501EB-9E24-4CAB-907B-4A5E7B3E6815}" name="Best for environment" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -953,7 +948,7 @@
   <autoFilter ref="J4:K8" xr:uid="{A37C58FD-0E87-422E-8B78-E0B60D39C0DC}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{22B7978F-E9E2-443D-9A73-AB8AADD6B6C5}" name="Env. Impact"/>
-    <tableColumn id="2" xr3:uid="{6022F85B-1298-4415-90E3-7D8DBC7DCF1B}" name="Fact name" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6022F85B-1298-4415-90E3-7D8DBC7DCF1B}" name="Fact name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1258,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE26F62-A483-48E5-AECB-A7F6D49F2DE9}">
   <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -1675,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B6D6D2-DF8F-42D4-B348-6064A7AEAE7C}">
-  <dimension ref="B4:K26"/>
+  <dimension ref="B4:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,6 +1794,9 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1885,12 +1883,32 @@
         <v>22</v>
       </c>
     </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G5:H7">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:K8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">

</xml_diff>